<commit_message>
Dodano zużycie do kondensatorów
</commit_message>
<xml_diff>
--- a/zestaw_dla_IV_LO_2018_v1.xlsx
+++ b/zestaw_dla_IV_LO_2018_v1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="103">
   <si>
     <t>typ</t>
   </si>
@@ -1902,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2277,7 +2277,9 @@
         <v>45</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
       <c r="H12" s="15">
         <v>1</v>
       </c>
@@ -2287,6 +2289,9 @@
       <c r="J12" s="20">
         <f t="shared" si="0"/>
         <v>0.99</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="165.6">

</xml_diff>

<commit_message>
do sprawdzenia czy wszystko dobrze
</commit_message>
<xml_diff>
--- a/zestaw_dla_IV_LO_2018_v1.xlsx
+++ b/zestaw_dla_IV_LO_2018_v1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
   <si>
     <t>typ</t>
   </si>
@@ -87,15 +87,6 @@
   </si>
   <si>
     <t>rezystory</t>
-  </si>
-  <si>
-    <t>Zestaw rezystorów SMD 0805 - 400szt.</t>
-  </si>
-  <si>
-    <t>https://botland.com.pl/rezystory-smd-0805/9604-zestaw-rezystorow-smd-0805-400szt.html</t>
-  </si>
-  <si>
-    <t>Zbiór 20 popularnych wartości rezystorów w małych obudowach, przydatnych w warsztacie zarówno robotyka jak i elektronika. W skład zestawu wchodzi po 20 sztuk elementów o następujących rezystancjach:</t>
   </si>
   <si>
     <t>Mikrokontroler AVR - ATmega328P-AU SMD</t>
@@ -196,19 +187,7 @@
 Kanały sterownika można połączyć aby otrzymać większą wydajność prądową</t>
   </si>
   <si>
-    <t>Kondensator ceramiczny 100nF/50V THT - 10szt.</t>
-  </si>
-  <si>
     <t>Kondensator ceramiczny</t>
-  </si>
-  <si>
-    <t>Kondensator ceramiczny przewlekany 100 nF / 50 V. Cena za 10 sztuk. Pojemność: 100 nF
-Maksymalne napięcie: 50 V
-Obudowa: THT - przewlekana
-Raster wyprowadzeń 2,54 mm</t>
-  </si>
-  <si>
-    <t>https://botland.com.pl/kondensatory-ceramiczne-dip/210-kondensator-ceramiczny-100nf50v-tht-10szt.html</t>
   </si>
   <si>
     <t>Stabilizator 5V 7805CD2T - SMD TO263</t>
@@ -434,6 +413,31 @@
   </si>
   <si>
     <t>cena łącznie max</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/zestaw-kondensatorow-ceramicznych-0805-190szt-i6819067595.html</t>
+  </si>
+  <si>
+    <t>Zestaw kondensatorów ceramicznych 0805 190szt.</t>
+  </si>
+  <si>
+    <t>Zestaw kondensatorów SMD 0805.
+W skład zestawu wchodzi 19 wartości w listkach po 10 sztuk każdej od 22 pF do 1000 nF</t>
+  </si>
+  <si>
+    <t>średnie</t>
+  </si>
+  <si>
+    <t>cena łącznie min</t>
+  </si>
+  <si>
+    <t>https://botland.com.pl/zestawy-rezystorow/536-zestaw-rezystorow-smd-0805-2500-szt.html?search_query=zestaw%20rezystorow&amp;results=103</t>
+  </si>
+  <si>
+    <t>Zestaw rezystorów SMD 0805 - 1500szt.</t>
+  </si>
+  <si>
+    <t>Zbiór 30 popularnych wartości rezystorów o tolerancji 5 % w obudowach SMD 0805,  przydatnych w warsztacie zarówno robotyka jak i elektronika. Rezystory są zapakowane w osobne, opisane torebki strunowe. Całość znajduje się w kartonowym pudełku, ułatwiającym przechowywanie.</t>
   </si>
 </sst>
 </file>
@@ -503,7 +507,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -530,17 +534,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -548,19 +541,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -571,7 +551,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -625,19 +605,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1175,86 +1168,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>119744</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>21771</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1416624</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>989</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="bigpic" descr="Zestaw rezystorów SMD 0805 - 400szt."/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4659087" y="22326600"/>
-          <a:ext cx="1296880" cy="1295399"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>87085</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1348867</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1262742</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1033" name="bigpic" descr="Kondensator ceramiczny 100nF/50V THT - 10szt."/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4626428" y="15022286"/>
-          <a:ext cx="1261782" cy="1262742"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>141514</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>1045028</xdr:rowOff>
@@ -1273,7 +1186,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1313,7 +1226,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1353,7 +1266,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1393,7 +1306,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1433,7 +1346,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1473,7 +1386,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1513,7 +1426,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1553,7 +1466,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1593,7 +1506,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1603,6 +1516,86 @@
         <a:xfrm>
           <a:off x="5015345" y="24328581"/>
           <a:ext cx="1427018" cy="1423567"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>166254</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>27710</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1454727</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1316366</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 1" descr="Zestaw kondensatorów ceramicznych 0805 190szt."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4710545" y="15544801"/>
+          <a:ext cx="1288473" cy="1288656"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1357745</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>37296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="bigpic" descr="Zestaw rezystorów SMD 0805 - 1500szt."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4544291" y="23026256"/>
+          <a:ext cx="1357745" cy="1353476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1900,10 +1893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1911,14 +1904,16 @@
     <col min="1" max="1" width="25.3984375" customWidth="1"/>
     <col min="2" max="4" width="34.09765625" customWidth="1"/>
     <col min="5" max="5" width="57.5" customWidth="1"/>
-    <col min="6" max="7" width="20.19921875" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" style="27" customWidth="1"/>
     <col min="8" max="8" width="8.796875" style="18"/>
     <col min="9" max="9" width="11.8984375" customWidth="1"/>
-    <col min="10" max="10" width="17.3984375" customWidth="1"/>
-    <col min="11" max="11" width="22.09765625" style="23" customWidth="1"/>
+    <col min="10" max="10" width="17.8984375" customWidth="1"/>
+    <col min="11" max="11" width="17.3984375" customWidth="1"/>
+    <col min="12" max="12" width="22.09765625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.2" customHeight="1">
+    <row r="1" spans="1:12" ht="19.2" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1938,36 +1933,39 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="L1" s="23" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="75.599999999999994" customHeight="1">
+    <row r="2" spans="1:12" ht="75.599999999999994" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="1">
+      <c r="G2" s="8">
         <v>1</v>
       </c>
       <c r="H2" s="15">
@@ -1976,29 +1974,33 @@
       <c r="I2" s="13">
         <v>0.5</v>
       </c>
-      <c r="J2" s="20">
-        <f t="shared" ref="J2:J16" si="0">H2*I2</f>
+      <c r="J2" s="24">
+        <f>G2*I2</f>
+        <v>0.5</v>
+      </c>
+      <c r="K2" s="20">
+        <f t="shared" ref="K2:K16" si="0">H2*I2</f>
         <v>1.5</v>
       </c>
-      <c r="K2" s="23" t="s">
-        <v>97</v>
+      <c r="L2" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="233.25" customHeight="1">
+    <row r="3" spans="1:12" ht="233.25" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="1">
+      <c r="G3" s="8">
         <v>4</v>
       </c>
       <c r="H3" s="15">
@@ -2007,29 +2009,33 @@
       <c r="I3" s="13">
         <v>1.2</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="24">
+        <f t="shared" ref="J3:J25" si="1">G3*I3</f>
+        <v>4.8</v>
+      </c>
+      <c r="K3" s="20">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="K3" s="23" t="s">
-        <v>98</v>
+      <c r="L3" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="67.2" customHeight="1">
+    <row r="4" spans="1:12" ht="67.2" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="1">
+      <c r="G4" s="8">
         <v>1</v>
       </c>
       <c r="H4" s="15">
@@ -2038,29 +2044,33 @@
       <c r="I4" s="13">
         <v>0.7</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="24">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="K4" s="20">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>98</v>
+      <c r="L4" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="61.5" customHeight="1">
+    <row r="5" spans="1:12" ht="61.5" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1">
+      <c r="G5" s="8">
         <v>1</v>
       </c>
       <c r="H5" s="15">
@@ -2069,29 +2079,33 @@
       <c r="I5" s="13">
         <v>0.7</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="24">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="K5" s="20">
         <f>H5*I5</f>
         <v>0.7</v>
       </c>
-      <c r="K5" s="23" t="s">
-        <v>98</v>
+      <c r="L5" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="70.5" customHeight="1">
+    <row r="6" spans="1:12" ht="70.5" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1">
+      <c r="G6" s="8">
         <v>1</v>
       </c>
       <c r="H6" s="15">
@@ -2100,29 +2114,33 @@
       <c r="I6" s="13">
         <v>0.8</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="24">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="20">
         <f>H6*I6</f>
         <v>0.8</v>
       </c>
-      <c r="K6" s="23" t="s">
-        <v>98</v>
+      <c r="L6" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="70.5" customHeight="1">
+    <row r="7" spans="1:12" ht="70.5" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1">
+      <c r="G7" s="8">
         <v>1</v>
       </c>
       <c r="H7" s="15">
@@ -2131,29 +2149,33 @@
       <c r="I7" s="13">
         <v>0.8</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="24">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="20">
         <f>H7*I7</f>
         <v>0.8</v>
       </c>
-      <c r="K7" s="23" t="s">
-        <v>99</v>
+      <c r="L7" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="54.6" customHeight="1">
+    <row r="8" spans="1:12" ht="54.6" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1">
+      <c r="G8" s="8">
         <v>1</v>
       </c>
       <c r="H8" s="15">
@@ -2162,29 +2184,33 @@
       <c r="I8" s="13">
         <v>0.8</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="24">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="20">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="K8" s="23" t="s">
-        <v>99</v>
+      <c r="L8" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="391.8" customHeight="1">
+    <row r="9" spans="1:12" ht="391.8" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1">
+      <c r="G9" s="8">
         <v>1</v>
       </c>
       <c r="H9" s="15">
@@ -2193,29 +2219,33 @@
       <c r="I9" s="13">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="24">
+        <f t="shared" si="1"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K9" s="20">
         <f t="shared" si="0"/>
         <v>4.9000000000000004</v>
       </c>
-      <c r="K9" s="23" t="s">
-        <v>98</v>
+      <c r="L9" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="82.8">
+    <row r="10" spans="1:12" ht="82.8">
       <c r="A10" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="1">
+      <c r="G10" s="8">
         <v>1</v>
       </c>
       <c r="H10" s="15">
@@ -2224,29 +2254,33 @@
       <c r="I10" s="13">
         <v>1.3</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="24">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="K10" s="20">
         <f t="shared" si="0"/>
         <v>3.9000000000000004</v>
       </c>
-      <c r="K10" s="23" t="s">
-        <v>97</v>
+      <c r="L10" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="96.6">
+    <row r="11" spans="1:12" ht="96.6">
       <c r="A11" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1">
+      <c r="G11" s="8">
         <v>1</v>
       </c>
       <c r="H11" s="15">
@@ -2255,151 +2289,194 @@
       <c r="I11" s="13">
         <v>0.9</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="24">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="K11" s="20">
         <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="L11" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="104.4" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>97</v>
       </c>
+      <c r="E12" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1</v>
+      </c>
+      <c r="I12" s="13">
+        <v>11.99</v>
+      </c>
+      <c r="J12" s="24">
+        <f t="shared" si="1"/>
+        <v>11.99</v>
+      </c>
+      <c r="K12" s="20">
+        <f t="shared" si="0"/>
+        <v>11.99</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" ht="104.4" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="15">
-        <v>1</v>
-      </c>
-      <c r="I12" s="13">
-        <v>0.99</v>
-      </c>
-      <c r="J12" s="20">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="165.6">
+    <row r="13" spans="1:12" ht="165.6">
       <c r="A13" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>25</v>
-      </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
       <c r="H13" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13" s="13">
         <v>8.9</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="24">
+        <f t="shared" si="1"/>
+        <v>8.9</v>
+      </c>
+      <c r="K13" s="20">
         <f t="shared" si="0"/>
-        <v>17.8</v>
+        <v>26.700000000000003</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="160.5" customHeight="1">
+    <row r="14" spans="1:12" ht="160.5" customHeight="1">
       <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
       <c r="H14" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I14" s="13">
         <v>10.9</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="24">
+        <f t="shared" si="1"/>
+        <v>10.9</v>
+      </c>
+      <c r="K14" s="20">
         <f t="shared" si="0"/>
-        <v>21.8</v>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="160.5" customHeight="1">
+    <row r="15" spans="1:12" ht="160.5" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
       <c r="H15" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="14">
         <v>2</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="24">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K15" s="20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="103.8" customHeight="1">
+    <row r="16" spans="1:12" ht="103.8" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="8"/>
+        <v>103</v>
+      </c>
       <c r="D16" s="9" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="8">
+        <v>1</v>
+      </c>
       <c r="H16" s="15">
         <v>1</v>
       </c>
       <c r="I16" s="13">
-        <v>11.9</v>
-      </c>
-      <c r="J16" s="20">
+        <v>23.9</v>
+      </c>
+      <c r="J16" s="24">
+        <f t="shared" si="1"/>
+        <v>23.9</v>
+      </c>
+      <c r="K16" s="20">
         <f t="shared" si="0"/>
-        <v>11.9</v>
+        <v>23.9</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="114.75" customHeight="1">
+    <row r="17" spans="1:12" ht="114.75" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -2412,49 +2489,64 @@
       <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="4">
-        <f>0.6*H17</f>
-        <v>3</v>
-      </c>
-      <c r="G17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="10">
+        <v>5</v>
+      </c>
       <c r="H17" s="17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I17" s="2">
         <v>28.41</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="24">
+        <f t="shared" si="1"/>
+        <v>142.05000000000001</v>
+      </c>
+      <c r="K17" s="20">
         <f>H17*I17</f>
-        <v>142.05000000000001</v>
+        <v>198.87</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="158.25" customHeight="1">
+    <row r="18" spans="1:12" ht="158.25" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="10">
+        <v>10</v>
+      </c>
       <c r="H18" s="17">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I18" s="2">
         <v>2.66</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="24">
+        <f t="shared" si="1"/>
+        <v>26.6</v>
+      </c>
+      <c r="K18" s="20">
         <f>H18*I18</f>
-        <v>26.6</v>
+        <v>31.92</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="172.5" customHeight="1">
+    <row r="19" spans="1:12" ht="172.5" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -2471,175 +2563,238 @@
         <f>4*10</f>
         <v>40</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="10">
+        <v>4</v>
+      </c>
       <c r="H19" s="17">
         <v>6</v>
       </c>
       <c r="I19" s="2">
         <v>61.66</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="24">
+        <f t="shared" si="1"/>
+        <v>246.64</v>
+      </c>
+      <c r="K19" s="20">
         <f>H19*I19</f>
         <v>369.96</v>
       </c>
+      <c r="L19" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" ht="172.5" customHeight="1">
+    <row r="20" spans="1:12" ht="172.5" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="10">
+        <v>1</v>
+      </c>
       <c r="H20" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I20" s="2">
         <v>8.9</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="24">
+        <f t="shared" si="1"/>
+        <v>8.9</v>
+      </c>
+      <c r="K20" s="20">
         <f>H20*I20</f>
-        <v>17.8</v>
+        <v>26.700000000000003</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="189" customHeight="1">
+    <row r="21" spans="1:12" ht="189" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F21" s="6">
         <v>43</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="25">
+        <v>2</v>
+      </c>
       <c r="H21" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I21" s="2">
         <v>24.9</v>
       </c>
-      <c r="J21" s="20">
-        <f t="shared" ref="J21:J25" si="1">H21*I21</f>
+      <c r="J21" s="24">
+        <f t="shared" si="1"/>
         <v>49.8</v>
       </c>
+      <c r="K21" s="20">
+        <f t="shared" ref="K21:K25" si="2">H21*I21</f>
+        <v>74.699999999999989</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" ht="189" customHeight="1">
+    <row r="22" spans="1:12" ht="189" customHeight="1">
       <c r="A22" s="12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="G22" s="25">
+        <v>1</v>
+      </c>
       <c r="H22" s="17">
         <v>1</v>
       </c>
       <c r="I22" s="2">
         <v>5.99</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="24">
         <f t="shared" si="1"/>
         <v>5.99</v>
       </c>
+      <c r="K22" s="20">
+        <f t="shared" si="2"/>
+        <v>5.99</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" ht="189" customHeight="1">
+    <row r="23" spans="1:12" ht="189" customHeight="1">
       <c r="A23" s="12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="G23" s="25">
+        <v>1</v>
+      </c>
       <c r="H23" s="17">
         <v>1</v>
       </c>
       <c r="I23" s="2">
         <v>5.95</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J23" s="24">
         <f t="shared" si="1"/>
         <v>5.95</v>
       </c>
+      <c r="K23" s="20">
+        <f t="shared" si="2"/>
+        <v>5.95</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" ht="189" customHeight="1">
+    <row r="24" spans="1:12" ht="189" customHeight="1">
       <c r="A24" s="12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="G24" s="25">
+        <v>1</v>
+      </c>
       <c r="H24" s="17">
         <v>1</v>
       </c>
       <c r="I24" s="2">
         <v>2.5</v>
       </c>
-      <c r="J24" s="20">
+      <c r="J24" s="24">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
+      <c r="K24" s="20">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="25" spans="1:10" ht="189" customHeight="1">
+    <row r="25" spans="1:12" ht="189" customHeight="1">
       <c r="A25" s="12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="G25" s="25">
+        <v>1</v>
+      </c>
       <c r="H25" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25" s="2">
         <v>0.8</v>
       </c>
-      <c r="J25" s="20">
+      <c r="J25" s="24">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="K25" s="20">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>12</v>
       </c>
@@ -2650,16 +2805,21 @@
         <v>17</v>
       </c>
       <c r="F26" s="7">
-        <f>SUM(F2:F21)</f>
-        <v>86</v>
-      </c>
-      <c r="G26" s="7"/>
+        <f>SUM(F2:F25)</f>
+        <v>83</v>
+      </c>
+      <c r="G26" s="26"/>
       <c r="H26" s="17"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="21">
-        <f>SUM(J2:J22)</f>
-        <v>688.29</v>
-      </c>
+      <c r="J26" s="28">
+        <f>SUM(J2:J25)</f>
+        <v>563.11999999999989</v>
+      </c>
+      <c r="K26" s="21">
+        <f>SUM(K2:K25)</f>
+        <v>839.08</v>
+      </c>
+      <c r="L26" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ostateczne sprawdzenie' git push origin master git status
</commit_message>
<xml_diff>
--- a/zestaw_dla_IV_LO_2018_v1.xlsx
+++ b/zestaw_dla_IV_LO_2018_v1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="106">
   <si>
     <t>typ</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Zbiór 30 popularnych wartości rezystorów o tolerancji 5 % w obudowach SMD 0805,  przydatnych w warsztacie zarówno robotyka jak i elektronika. Rezystory są zapakowane w osobne, opisane torebki strunowe. Całość znajduje się w kartonowym pudełku, ułatwiającym przechowywanie.</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,6 +506,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +560,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -570,9 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,12 +614,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -626,11 +626,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1895,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="F17" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1905,12 +1911,12 @@
     <col min="2" max="4" width="34.09765625" customWidth="1"/>
     <col min="5" max="5" width="57.5" customWidth="1"/>
     <col min="6" max="6" width="20.19921875" customWidth="1"/>
-    <col min="7" max="7" width="20.19921875" style="27" customWidth="1"/>
-    <col min="8" max="8" width="8.796875" style="18"/>
-    <col min="9" max="9" width="11.8984375" customWidth="1"/>
-    <col min="10" max="10" width="17.8984375" customWidth="1"/>
-    <col min="11" max="11" width="17.3984375" customWidth="1"/>
-    <col min="12" max="12" width="22.09765625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="22.09765625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="14.19921875" style="23" customWidth="1"/>
+    <col min="9" max="9" width="10.59765625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="11.8984375" customWidth="1"/>
+    <col min="11" max="11" width="17.8984375" customWidth="1"/>
+    <col min="12" max="12" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19.2" customHeight="1">
@@ -1932,548 +1938,578 @@
       <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="75.599999999999994" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="8">
-        <v>1</v>
-      </c>
-      <c r="H2" s="15">
+      <c r="F2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1</v>
+      </c>
+      <c r="I2" s="14">
         <v>3</v>
       </c>
-      <c r="I2" s="13">
+      <c r="J2" s="12">
         <v>0.5</v>
       </c>
-      <c r="J2" s="24">
-        <f>G2*I2</f>
+      <c r="K2" s="21">
+        <f>H2*J2</f>
         <v>0.5</v>
       </c>
-      <c r="K2" s="20">
-        <f t="shared" ref="K2:K16" si="0">H2*I2</f>
+      <c r="L2" s="2">
+        <f>J2*I2</f>
         <v>1.5</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="233.25" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="8">
+      <c r="F3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="7">
         <v>4</v>
       </c>
-      <c r="H3" s="15">
+      <c r="I3" s="14">
         <v>4</v>
       </c>
-      <c r="I3" s="13">
+      <c r="J3" s="12">
         <v>1.2</v>
       </c>
-      <c r="J3" s="24">
-        <f t="shared" ref="J3:J25" si="1">G3*I3</f>
+      <c r="K3" s="21">
+        <f>H3*J3</f>
         <v>4.8</v>
       </c>
-      <c r="K3" s="20">
-        <f t="shared" si="0"/>
+      <c r="L3" s="2">
+        <f>I3*J3</f>
         <v>4.8</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="67.2" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="8">
-        <v>1</v>
-      </c>
-      <c r="H4" s="15">
-        <v>1</v>
-      </c>
-      <c r="I4" s="13">
+      <c r="F4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1</v>
+      </c>
+      <c r="J4" s="12">
         <v>0.7</v>
       </c>
-      <c r="J4" s="24">
-        <f t="shared" si="1"/>
+      <c r="K4" s="21">
+        <f>H4*J4</f>
         <v>0.7</v>
       </c>
-      <c r="K4" s="20">
-        <f t="shared" si="0"/>
+      <c r="L4" s="2">
+        <f>I4*J4</f>
         <v>0.7</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="61.5" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="8">
-        <v>1</v>
-      </c>
-      <c r="H5" s="15">
-        <v>1</v>
-      </c>
-      <c r="I5" s="13">
+      <c r="F5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1</v>
+      </c>
+      <c r="J5" s="12">
         <v>0.7</v>
       </c>
-      <c r="J5" s="24">
-        <f t="shared" si="1"/>
+      <c r="K5" s="21">
+        <f>H5*J5</f>
         <v>0.7</v>
       </c>
-      <c r="K5" s="20">
-        <f>H5*I5</f>
+      <c r="L5" s="2">
+        <f>I5*J5</f>
         <v>0.7</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="70.5" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
-      <c r="H6" s="15">
-        <v>1</v>
-      </c>
-      <c r="I6" s="13">
+      <c r="F6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+      <c r="J6" s="12">
         <v>0.8</v>
       </c>
-      <c r="J6" s="24">
-        <f t="shared" si="1"/>
+      <c r="K6" s="21">
+        <f>H6*J6</f>
         <v>0.8</v>
       </c>
-      <c r="K6" s="20">
-        <f>H6*I6</f>
+      <c r="L6" s="2">
+        <f>I6*J6</f>
         <v>0.8</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="70.5" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="15">
-        <v>1</v>
-      </c>
-      <c r="I7" s="13">
+      <c r="F7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="14">
+        <v>1</v>
+      </c>
+      <c r="J7" s="12">
         <v>0.8</v>
       </c>
-      <c r="J7" s="24">
-        <f t="shared" si="1"/>
+      <c r="K7" s="21">
+        <f>H7*J7</f>
         <v>0.8</v>
       </c>
-      <c r="K7" s="20">
-        <f>H7*I7</f>
+      <c r="L7" s="2">
+        <f>I7*J7</f>
         <v>0.8</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="54.6" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="15">
-        <v>1</v>
-      </c>
-      <c r="I8" s="13">
+      <c r="F8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="14">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12">
         <v>0.8</v>
       </c>
-      <c r="J8" s="24">
-        <f t="shared" si="1"/>
+      <c r="K8" s="21">
+        <f>H8*J8</f>
         <v>0.8</v>
       </c>
-      <c r="K8" s="20">
-        <f t="shared" si="0"/>
+      <c r="L8" s="2">
+        <f>I8*J8</f>
         <v>0.8</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="391.8" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="15">
-        <v>1</v>
-      </c>
-      <c r="I9" s="13">
+      <c r="F9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J9" s="24">
-        <f t="shared" si="1"/>
+      <c r="K9" s="21">
+        <f>H9*J9</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="K9" s="20">
-        <f t="shared" si="0"/>
+      <c r="L9" s="2">
+        <f>I9*J9</f>
         <v>4.9000000000000004</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="82.8">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="8">
-        <v>1</v>
-      </c>
-      <c r="H10" s="15">
+      <c r="F10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="14">
         <v>3</v>
       </c>
-      <c r="I10" s="13">
+      <c r="J10" s="12">
         <v>1.3</v>
       </c>
-      <c r="J10" s="24">
-        <f t="shared" si="1"/>
+      <c r="K10" s="21">
+        <f>H10*J10</f>
         <v>1.3</v>
       </c>
-      <c r="K10" s="20">
-        <f t="shared" si="0"/>
+      <c r="L10" s="2">
+        <f>I10*J10</f>
         <v>3.9000000000000004</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="96.6">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="8">
-        <v>1</v>
-      </c>
-      <c r="H11" s="15">
+      <c r="F11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="14">
         <v>3</v>
       </c>
-      <c r="I11" s="13">
+      <c r="J11" s="12">
         <v>0.9</v>
       </c>
-      <c r="J11" s="24">
-        <f t="shared" si="1"/>
+      <c r="K11" s="21">
+        <f>H11*J11</f>
         <v>0.9</v>
       </c>
-      <c r="K11" s="20">
-        <f t="shared" si="0"/>
+      <c r="L11" s="2">
+        <f>I11*J11</f>
         <v>2.7</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="104.4" customHeight="1">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="8">
-        <v>1</v>
-      </c>
-      <c r="H12" s="15">
-        <v>1</v>
-      </c>
-      <c r="I12" s="13">
+      <c r="F12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14">
+        <v>1</v>
+      </c>
+      <c r="J12" s="12">
         <v>11.99</v>
       </c>
-      <c r="J12" s="24">
-        <f t="shared" si="1"/>
+      <c r="K12" s="21">
+        <f>H12*J12</f>
         <v>11.99</v>
       </c>
-      <c r="K12" s="20">
-        <f t="shared" si="0"/>
+      <c r="L12" s="2">
+        <f>I12*J12</f>
         <v>11.99</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="165.6">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
-      <c r="H13" s="15">
+      <c r="F13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1</v>
+      </c>
+      <c r="I13" s="14">
         <v>3</v>
       </c>
-      <c r="I13" s="13">
+      <c r="J13" s="12">
         <v>8.9</v>
       </c>
-      <c r="J13" s="24">
-        <f t="shared" si="1"/>
+      <c r="K13" s="21">
+        <f>H13*J13</f>
         <v>8.9</v>
       </c>
-      <c r="K13" s="20">
-        <f t="shared" si="0"/>
+      <c r="L13" s="2">
+        <f>I13*J13</f>
         <v>26.700000000000003</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="160.5" customHeight="1">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
-      <c r="H14" s="15">
+      <c r="F14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
+      <c r="I14" s="14">
         <v>3</v>
       </c>
-      <c r="I14" s="13">
+      <c r="J14" s="12">
         <v>10.9</v>
       </c>
-      <c r="J14" s="24">
-        <f t="shared" si="1"/>
+      <c r="K14" s="21">
+        <f>H14*J14</f>
         <v>10.9</v>
       </c>
-      <c r="K14" s="20">
-        <f t="shared" si="0"/>
+      <c r="L14" s="2">
+        <f>I14*J14</f>
         <v>32.700000000000003</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="160.5" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="8">
-        <v>1</v>
-      </c>
-      <c r="H15" s="15">
+      <c r="F15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="7">
+        <v>1</v>
+      </c>
+      <c r="I15" s="14">
+        <v>1</v>
+      </c>
+      <c r="J15" s="13">
         <v>2</v>
       </c>
-      <c r="I15" s="14">
+      <c r="K15" s="21">
+        <f>H15*J15</f>
         <v>2</v>
       </c>
-      <c r="J15" s="24">
-        <f t="shared" si="1"/>
+      <c r="L15" s="2">
+        <f>I15*J15</f>
         <v>2</v>
-      </c>
-      <c r="K15" s="20">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="103.8" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="8">
-        <v>1</v>
-      </c>
-      <c r="H16" s="15">
-        <v>1</v>
-      </c>
-      <c r="I16" s="13">
+      <c r="F16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1</v>
+      </c>
+      <c r="I16" s="14">
+        <v>1</v>
+      </c>
+      <c r="J16" s="12">
         <v>23.9</v>
       </c>
-      <c r="J16" s="24">
-        <f t="shared" si="1"/>
+      <c r="K16" s="21">
+        <f>H16*J16</f>
         <v>23.9</v>
       </c>
-      <c r="K16" s="20">
-        <f t="shared" si="0"/>
+      <c r="L16" s="2">
+        <f>I16*J16</f>
         <v>23.9</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="114.75" customHeight="1">
@@ -2489,26 +2525,28 @@
       <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="10">
-        <v>5</v>
-      </c>
-      <c r="H17" s="17">
-        <v>7</v>
-      </c>
-      <c r="I17" s="2">
+      <c r="F17" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="9">
+        <v>6</v>
+      </c>
+      <c r="I17" s="16">
+        <v>8</v>
+      </c>
+      <c r="J17" s="2">
         <v>28.41</v>
       </c>
-      <c r="J17" s="24">
-        <f t="shared" si="1"/>
-        <v>142.05000000000001</v>
-      </c>
-      <c r="K17" s="20">
-        <f>H17*I17</f>
-        <v>198.87</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>100</v>
+      <c r="K17" s="21">
+        <f>H17*J17</f>
+        <v>170.46</v>
+      </c>
+      <c r="L17" s="2">
+        <f>I17*J17</f>
+        <v>227.28</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="158.25" customHeight="1">
@@ -2524,26 +2562,28 @@
       <c r="E18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="10">
+      <c r="F18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="9">
         <v>10</v>
       </c>
-      <c r="H18" s="17">
+      <c r="I18" s="16">
         <v>12</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>2.66</v>
       </c>
-      <c r="J18" s="24">
-        <f t="shared" si="1"/>
+      <c r="K18" s="21">
+        <f>H18*J18</f>
         <v>26.6</v>
       </c>
-      <c r="K18" s="20">
-        <f>H18*I18</f>
+      <c r="L18" s="2">
+        <f>I18*J18</f>
         <v>31.92</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="172.5" customHeight="1">
@@ -2563,25 +2603,25 @@
         <f>4*10</f>
         <v>40</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="9">
         <v>4</v>
       </c>
-      <c r="H19" s="17">
+      <c r="I19" s="16">
         <v>6</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>61.66</v>
       </c>
-      <c r="J19" s="24">
-        <f t="shared" si="1"/>
+      <c r="K19" s="21">
+        <f>H19*J19</f>
         <v>246.64</v>
       </c>
-      <c r="K19" s="20">
-        <f>H19*I19</f>
+      <c r="L19" s="2">
+        <f>I19*J19</f>
         <v>369.96</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="172.5" customHeight="1">
@@ -2597,26 +2637,28 @@
       <c r="E20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="10">
-        <v>1</v>
-      </c>
-      <c r="H20" s="17">
+      <c r="F20" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1</v>
+      </c>
+      <c r="I20" s="16">
         <v>3</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>8.9</v>
       </c>
-      <c r="J20" s="24">
-        <f t="shared" si="1"/>
+      <c r="K20" s="21">
+        <f>H20*J20</f>
         <v>8.9</v>
       </c>
-      <c r="K20" s="20">
-        <f>H20*I20</f>
+      <c r="L20" s="2">
+        <f>I20*J20</f>
         <v>26.700000000000003</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="189" customHeight="1">
@@ -2626,7 +2668,7 @@
       <c r="B21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E21" s="6" t="s">
@@ -2635,99 +2677,103 @@
       <c r="F21" s="6">
         <v>43</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="22">
         <v>2</v>
       </c>
-      <c r="H21" s="17">
+      <c r="I21" s="16">
         <v>3</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>24.9</v>
       </c>
-      <c r="J21" s="24">
-        <f t="shared" si="1"/>
+      <c r="K21" s="21">
+        <f>H21*J21</f>
         <v>49.8</v>
       </c>
-      <c r="K21" s="20">
-        <f t="shared" ref="K21:K25" si="2">H21*I21</f>
+      <c r="L21" s="2">
+        <f>I21*J21</f>
         <v>74.699999999999989</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="189" customHeight="1">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="25">
-        <v>1</v>
-      </c>
-      <c r="H22" s="17">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2">
+      <c r="F22" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="16">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
         <v>5.99</v>
       </c>
-      <c r="J22" s="24">
-        <f t="shared" si="1"/>
+      <c r="K22" s="21">
+        <f>H22*J22</f>
         <v>5.99</v>
       </c>
-      <c r="K22" s="20">
-        <f t="shared" si="2"/>
+      <c r="L22" s="2">
+        <f>I22*J22</f>
         <v>5.99</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="189" customHeight="1">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>88</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="25">
-        <v>1</v>
-      </c>
-      <c r="H23" s="17">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
+      <c r="F23" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="22">
+        <v>1</v>
+      </c>
+      <c r="I23" s="16">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
         <v>5.95</v>
       </c>
-      <c r="J23" s="24">
-        <f t="shared" si="1"/>
+      <c r="K23" s="21">
+        <f>H23*J23</f>
         <v>5.95</v>
       </c>
-      <c r="K23" s="20">
-        <f t="shared" si="2"/>
+      <c r="L23" s="2">
+        <f>I23*J23</f>
         <v>5.95</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="189" customHeight="1">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -2739,30 +2785,32 @@
       <c r="E24" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="25">
-        <v>1</v>
-      </c>
-      <c r="H24" s="17">
-        <v>1</v>
-      </c>
-      <c r="I24" s="2">
+      <c r="F24" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="22">
+        <v>1</v>
+      </c>
+      <c r="I24" s="16">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
         <v>2.5</v>
       </c>
-      <c r="J24" s="24">
-        <f t="shared" si="1"/>
+      <c r="K24" s="21">
+        <f>H24*J24</f>
         <v>2.5</v>
       </c>
-      <c r="K24" s="20">
-        <f t="shared" si="2"/>
+      <c r="L24" s="2">
+        <f>I24*J24</f>
         <v>2.5</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="189" customHeight="1">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>73</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2772,26 +2820,28 @@
         <v>74</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="25">
-        <v>1</v>
-      </c>
-      <c r="H25" s="17">
+      <c r="F25" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" s="22">
         <v>2</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="16">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2">
         <v>0.8</v>
       </c>
-      <c r="J25" s="24">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="K25" s="20">
-        <f t="shared" si="2"/>
+      <c r="K25" s="21">
+        <f>H25*J25</f>
         <v>1.6</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>100</v>
+      <c r="L25" s="2">
+        <f>I25*J25</f>
+        <v>1.6</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2804,22 +2854,19 @@
       <c r="E26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="7">
-        <f>SUM(F2:F25)</f>
-        <v>83</v>
-      </c>
-      <c r="G26" s="26"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="28">
-        <f>SUM(J2:J25)</f>
-        <v>563.11999999999989</v>
-      </c>
-      <c r="K26" s="21">
+      <c r="F26" s="25"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="24">
         <f>SUM(K2:K25)</f>
-        <v>839.08</v>
-      </c>
-      <c r="L26" s="3"/>
+        <v>592.33000000000004</v>
+      </c>
+      <c r="L26" s="27">
+        <f>SUM(L2:L25)</f>
+        <v>865.49000000000012</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>